<commit_message>
finished LIAR ran, pretty much random guessing
</commit_message>
<xml_diff>
--- a/outputs/SA/LIAR_RESULTS.xlsx
+++ b/outputs/SA/LIAR_RESULTS.xlsx
@@ -502,10 +502,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7875</v>
+        <v>0.7699276090369407</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6182</v>
+        <v>0.620691213420634</v>
       </c>
     </row>
     <row r="3">
@@ -515,10 +515,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9074</v>
+        <v>0.9055856111439768</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6173999999999999</v>
+        <v>0.6316751175581654</v>
       </c>
     </row>
     <row r="4">
@@ -528,10 +528,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9085000000000001</v>
+        <v>0.9072389263485195</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6266</v>
+        <v>0.6341554327109823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>